<commit_message>
added average deadline to matlab script and results
</commit_message>
<xml_diff>
--- a/results_others.xlsx
+++ b/results_others.xlsx
@@ -859,15 +859,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J1" sqref="J1:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -895,8 +895,14 @@
       <c r="I1">
         <v>0.140698462796224</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>34.716666666666697</v>
+      </c>
+      <c r="K1">
+        <v>3.4986276566999801</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -924,8 +930,14 @@
       <c r="I2">
         <v>0.119584244179173</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>43.35</v>
+      </c>
+      <c r="K2">
+        <v>9.5132824184337892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -953,8 +965,14 @@
       <c r="I3">
         <v>0.14524087341981701</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>47.266666666666701</v>
+      </c>
+      <c r="K3">
+        <v>4.1451080690320703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -982,8 +1000,14 @@
       <c r="I4">
         <v>8.7403679220287606E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>40.133333333333297</v>
+      </c>
+      <c r="K4">
+        <v>5.8410199558205402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1011,8 +1035,14 @@
       <c r="I5">
         <v>0.14827229235306499</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>44.133333333333297</v>
+      </c>
+      <c r="K5">
+        <v>5.2544304684735001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1040,8 +1070,14 @@
       <c r="I6">
         <v>0.24046671553718801</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>52.016666666666701</v>
+      </c>
+      <c r="K6">
+        <v>5.5218876245223498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1069,8 +1105,14 @@
       <c r="I7">
         <v>0.16128347102851401</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>57.6666666666667</v>
+      </c>
+      <c r="K7">
+        <v>1.4458200027064201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1098,8 +1140,14 @@
       <c r="I8">
         <v>0.11768171344523699</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>45.766666666666701</v>
+      </c>
+      <c r="K8">
+        <v>2.31697250348831</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1127,8 +1175,14 @@
       <c r="I9">
         <v>7.2149798129007306E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>14.0833333333333</v>
+      </c>
+      <c r="K9">
+        <v>10.4058192107266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1156,8 +1210,14 @@
       <c r="I10">
         <v>0.27636650350555703</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>21.483333333333299</v>
+      </c>
+      <c r="K10">
+        <v>14.925227950638799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1185,8 +1245,14 @@
       <c r="I11">
         <v>8.6197758531293703E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>48.35</v>
+      </c>
+      <c r="K11">
+        <v>3.1880337705290902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1214,8 +1280,14 @@
       <c r="I12">
         <v>0.19333118992509499</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>50.1666666666667</v>
+      </c>
+      <c r="K12">
+        <v>6.1593711616807596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1243,8 +1315,14 @@
       <c r="I13">
         <v>8.2626755946707903E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>43.966666666666697</v>
+      </c>
+      <c r="K13">
+        <v>7.9040145703106797</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1272,8 +1350,14 @@
       <c r="I14">
         <v>9.6702757425236194E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>56.966666666666697</v>
+      </c>
+      <c r="K14">
+        <v>1.54004915909505</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1301,8 +1385,14 @@
       <c r="I15">
         <v>7.1559759444476997E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>42.45</v>
+      </c>
+      <c r="K15">
+        <v>2.7085864723072999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1330,8 +1420,14 @@
       <c r="I16">
         <v>7.3344934068818396E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>24.05</v>
+      </c>
+      <c r="K16">
+        <v>10.6809270847539</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1359,8 +1455,14 @@
       <c r="I17">
         <v>0.179577383494369</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>33.516666666666701</v>
+      </c>
+      <c r="K17">
+        <v>15.001120485457401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1388,8 +1490,14 @@
       <c r="I18">
         <v>0.16595894938615399</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>51.533333333333303</v>
+      </c>
+      <c r="K18">
+        <v>5.8843851590939398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1417,8 +1525,14 @@
       <c r="I19">
         <v>5.6707857495191201E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>32.283333333333303</v>
+      </c>
+      <c r="K19">
+        <v>6.0983233779948796</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1446,8 +1560,14 @@
       <c r="I20">
         <v>0.14857762555168399</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>52.466666666666697</v>
+      </c>
+      <c r="K20">
+        <v>5.7709578756268796</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1475,8 +1595,14 @@
       <c r="I21">
         <v>0.105991615591413</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>48.066666666666698</v>
+      </c>
+      <c r="K21">
+        <v>3.3133866471401001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1504,8 +1630,14 @@
       <c r="I22">
         <v>9.8109946635319897E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>53.616666666666703</v>
+      </c>
+      <c r="K22">
+        <v>5.5206597083880498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1533,8 +1665,14 @@
       <c r="I23">
         <v>0.10460243624365199</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>25.533333333333299</v>
+      </c>
+      <c r="K23">
+        <v>13.853307341345801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1562,8 +1700,14 @@
       <c r="I24">
         <v>0.195282334988713</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>51.783333333333303</v>
+      </c>
+      <c r="K24">
+        <v>2.4570318780425899</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1591,8 +1735,14 @@
       <c r="I25">
         <v>1.1165160779226999E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>2.6666666666666701</v>
+      </c>
+      <c r="K25">
+        <v>0.47538268854152799</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1620,8 +1770,14 @@
       <c r="I26">
         <v>0.13117533760157399</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>41.133333333333297</v>
+      </c>
+      <c r="K26">
+        <v>6.02105533479246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1649,8 +1805,14 @@
       <c r="I27">
         <v>0.10294395992508</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>56.566666666666698</v>
+      </c>
+      <c r="K27">
+        <v>1.3575484717340101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1677,6 +1839,12 @@
       </c>
       <c r="I28">
         <v>6.9381751737213296E-2</v>
+      </c>
+      <c r="J28">
+        <v>41.383333333333297</v>
+      </c>
+      <c r="K28">
+        <v>2.3512828569626301</v>
       </c>
     </row>
   </sheetData>
@@ -1686,15 +1854,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I36"/>
+      <selection activeCell="J1" sqref="J1:K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1722,8 +1890,14 @@
       <c r="I1">
         <v>9.4312404228029306E-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>99.383333333333297</v>
+      </c>
+      <c r="K1">
+        <v>32.360831978298798</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1751,8 +1925,14 @@
       <c r="I2">
         <v>0.148153373600308</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>94.8</v>
+      </c>
+      <c r="K2">
+        <v>17.4810308814431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1780,8 +1960,14 @@
       <c r="I3">
         <v>9.5897035649323795E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>69.75</v>
+      </c>
+      <c r="K3">
+        <v>46.114310804965399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1809,8 +1995,14 @@
       <c r="I4">
         <v>7.9855274341052399E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>60.05</v>
+      </c>
+      <c r="K4">
+        <v>18.742162203646501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1838,8 +2030,14 @@
       <c r="I5">
         <v>5.5317489510411301E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>95.266666666666694</v>
+      </c>
+      <c r="K5">
+        <v>16.491257742237401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1867,8 +2065,14 @@
       <c r="I6">
         <v>7.3684314281658295E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>89.366666666666703</v>
+      </c>
+      <c r="K6">
+        <v>10.697642171179499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1896,8 +2100,14 @@
       <c r="I7">
         <v>5.8139427574829199E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>81.866666666666703</v>
+      </c>
+      <c r="K7">
+        <v>12.512321610732201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1925,8 +2135,14 @@
       <c r="I8">
         <v>5.3287133207029699E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>115.433333333333</v>
+      </c>
+      <c r="K8">
+        <v>28.9835527098321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1954,8 +2170,14 @@
       <c r="I9">
         <v>8.3520064894610793E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>67.4166666666667</v>
+      </c>
+      <c r="K9">
+        <v>17.242332284202998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1983,8 +2205,14 @@
       <c r="I10">
         <v>0.133098726432123</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>103.26666666666701</v>
+      </c>
+      <c r="K10">
+        <v>29.105807368957699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2012,8 +2240,14 @@
       <c r="I11">
         <v>0.100893591737256</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="K11">
+        <v>34.679549974598501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2041,8 +2275,14 @@
       <c r="I12">
         <v>5.86132152476442E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="K12">
+        <v>34.742003103750598</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2070,8 +2310,14 @@
       <c r="I13">
         <v>8.6377106471244094E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>62.1666666666667</v>
+      </c>
+      <c r="K13">
+        <v>24.257912681919201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2099,8 +2345,14 @@
       <c r="I14">
         <v>7.8349249314255395E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="K14">
+        <v>18.417659175137501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2128,8 +2380,14 @@
       <c r="I15">
         <v>8.8449932159290298E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>93.983333333333306</v>
+      </c>
+      <c r="K15">
+        <v>49.518184184920898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2157,8 +2415,14 @@
       <c r="I16">
         <v>6.9565233047107003E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>41.8333333333333</v>
+      </c>
+      <c r="K16">
+        <v>11.1601085388481</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2186,8 +2450,14 @@
       <c r="I17">
         <v>0.113958781570223</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>108.566666666667</v>
+      </c>
+      <c r="K17">
+        <v>16.031078573383301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2215,8 +2485,14 @@
       <c r="I18">
         <v>0.112803210811477</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>56.6</v>
+      </c>
+      <c r="K18">
+        <v>49.901326363949103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2244,8 +2520,14 @@
       <c r="I19">
         <v>9.2584730162666606E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>99.8</v>
+      </c>
+      <c r="K19">
+        <v>14.072210865534499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2273,8 +2555,14 @@
       <c r="I20">
         <v>8.9880651364559597E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>97.266666666666694</v>
+      </c>
+      <c r="K20">
+        <v>18.121872416696</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2302,8 +2590,14 @@
       <c r="I21">
         <v>8.6395244641021302E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>136.38333333333301</v>
+      </c>
+      <c r="K21">
+        <v>18.4823247369917</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2331,8 +2625,14 @@
       <c r="I22">
         <v>7.6301077700810294E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>72.766666666666694</v>
+      </c>
+      <c r="K22">
+        <v>30.360750011205901</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2360,8 +2660,14 @@
       <c r="I23">
         <v>0.121234976204288</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>105.383333333333</v>
+      </c>
+      <c r="K23">
+        <v>29.4498088777814</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2389,8 +2695,14 @@
       <c r="I24">
         <v>9.9563322290161405E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>109.633333333333</v>
+      </c>
+      <c r="K24">
+        <v>45.5113942397914</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2418,8 +2730,14 @@
       <c r="I25">
         <v>8.1816791132818104E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>87.9</v>
+      </c>
+      <c r="K25">
+        <v>12.942768414728301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2447,8 +2765,14 @@
       <c r="I26">
         <v>9.3921777444194707E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>169.833333333333</v>
+      </c>
+      <c r="K26">
+        <v>2.9754171715295299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2476,8 +2800,14 @@
       <c r="I27">
         <v>8.2000124854528095E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>67.216666666666697</v>
+      </c>
+      <c r="K27">
+        <v>19.692631046006099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2505,8 +2835,14 @@
       <c r="I28">
         <v>0.15189093402384601</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>108.2</v>
+      </c>
+      <c r="K28">
+        <v>14.616916134675501</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2534,8 +2870,14 @@
       <c r="I29">
         <v>0.14189490307063299</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>99.9166666666667</v>
+      </c>
+      <c r="K29">
+        <v>28.9279008282261</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2563,8 +2905,14 @@
       <c r="I30">
         <v>6.6627322177654505E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>118.65</v>
+      </c>
+      <c r="K30">
+        <v>27.982939717875201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2592,8 +2940,14 @@
       <c r="I31">
         <v>9.9709689742568802E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>75.7</v>
+      </c>
+      <c r="K31">
+        <v>15.714939453714001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2621,8 +2975,14 @@
       <c r="I32">
         <v>0.14081386426378001</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>133.51666666666699</v>
+      </c>
+      <c r="K32">
+        <v>30.437761820356801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2650,8 +3010,14 @@
       <c r="I33">
         <v>0.15833334107815</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>132.01666666666699</v>
+      </c>
+      <c r="K33">
+        <v>47.110577338588598</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2679,8 +3045,14 @@
       <c r="I34">
         <v>0.10945093241763799</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>98.1666666666667</v>
+      </c>
+      <c r="K34">
+        <v>45.685426473771599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2708,8 +3080,14 @@
       <c r="I35">
         <v>0.14234083524392399</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>97.366666666666703</v>
+      </c>
+      <c r="K35">
+        <v>32.678177379348398</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -2736,6 +3114,12 @@
       </c>
       <c r="I36">
         <v>0.105062748922528</v>
+      </c>
+      <c r="J36">
+        <v>41.0833333333333</v>
+      </c>
+      <c r="K36">
+        <v>40.079705193047303</v>
       </c>
     </row>
   </sheetData>
@@ -2745,15 +3129,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I35"/>
+      <selection activeCell="J1" sqref="J1:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2781,8 +3165,14 @@
       <c r="I1">
         <v>7.2866325140959504E-2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>99.616666666666703</v>
+      </c>
+      <c r="K1">
+        <v>18.8185732871802</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2810,8 +3200,14 @@
       <c r="I2">
         <v>8.9228562840130698E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>119.916666666667</v>
+      </c>
+      <c r="K2">
+        <v>25.333231117843098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2839,8 +3235,14 @@
       <c r="I3">
         <v>9.6063945447810897E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>102.783333333333</v>
+      </c>
+      <c r="K3">
+        <v>8.5788302048482006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2868,8 +3270,14 @@
       <c r="I4">
         <v>7.9684926114231405E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>128.53333333333299</v>
+      </c>
+      <c r="K4">
+        <v>7.8620881054927798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2897,8 +3305,14 @@
       <c r="I5">
         <v>5.4595077057094203E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>104.933333333333</v>
+      </c>
+      <c r="K5">
+        <v>10.881280250366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2926,8 +3340,14 @@
       <c r="I6">
         <v>8.2950581080435598E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>106.35</v>
+      </c>
+      <c r="K6">
+        <v>8.35205242207069</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2955,8 +3375,14 @@
       <c r="I7">
         <v>7.36306490432556E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>162.25</v>
+      </c>
+      <c r="K7">
+        <v>5.4169382808910704</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2984,8 +3410,14 @@
       <c r="I8">
         <v>9.5662414263302104E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>101.4</v>
+      </c>
+      <c r="K8">
+        <v>7.4017863166918101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -3013,8 +3445,14 @@
       <c r="I9">
         <v>6.8743524467712105E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>143.80000000000001</v>
+      </c>
+      <c r="K9">
+        <v>24.130857943403999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -3042,8 +3480,14 @@
       <c r="I10">
         <v>9.69735037263878E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>97.183333333333294</v>
+      </c>
+      <c r="K10">
+        <v>37.0054927973557</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -3071,8 +3515,14 @@
       <c r="I11">
         <v>8.86828121480156E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="K11">
+        <v>10.110910368239701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -3100,8 +3550,14 @@
       <c r="I12">
         <v>7.4617564566123895E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>104.51666666666701</v>
+      </c>
+      <c r="K12">
+        <v>13.011717882735001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -3129,8 +3585,14 @@
       <c r="I13">
         <v>7.3877841283894893E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>101.666666666667</v>
+      </c>
+      <c r="K13">
+        <v>7.4188643350986601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -3158,8 +3620,14 @@
       <c r="I14">
         <v>5.1615923988169998E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>165.1</v>
+      </c>
+      <c r="K14">
+        <v>4.5349864051521998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -3187,8 +3655,14 @@
       <c r="I15">
         <v>0.106746411558655</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>79.75</v>
+      </c>
+      <c r="K15">
+        <v>14.240816249696801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -3216,8 +3690,14 @@
       <c r="I16">
         <v>5.6563249896642701E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>115.683333333333</v>
+      </c>
+      <c r="K16">
+        <v>18.450567642424499</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -3245,8 +3725,14 @@
       <c r="I17">
         <v>0.12475332172355399</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>128.38333333333301</v>
+      </c>
+      <c r="K17">
+        <v>7.0086911340441702</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -3274,8 +3760,14 @@
       <c r="I18">
         <v>7.8940631526247099E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>127.216666666667</v>
+      </c>
+      <c r="K18">
+        <v>7.7088803440053599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -3303,8 +3795,14 @@
       <c r="I19">
         <v>7.5883391521368498E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>129.01666666666699</v>
+      </c>
+      <c r="K19">
+        <v>9.2415635676621992</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -3332,8 +3830,14 @@
       <c r="I20">
         <v>0.10837382889507299</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>163.05000000000001</v>
+      </c>
+      <c r="K20">
+        <v>3.4268382423136101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -3361,8 +3865,14 @@
       <c r="I21">
         <v>9.2861550710241395E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>125.166666666667</v>
+      </c>
+      <c r="K21">
+        <v>8.7936160716635303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -3390,8 +3900,14 @@
       <c r="I22">
         <v>8.5370411397977297E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>126.916666666667</v>
+      </c>
+      <c r="K22">
+        <v>31.6523979152498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -3419,8 +3935,14 @@
       <c r="I23">
         <v>9.1267267801604005E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>104.133333333333</v>
+      </c>
+      <c r="K23">
+        <v>9.05438683202539</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -3448,8 +3970,14 @@
       <c r="I24">
         <v>6.3118491336210794E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>161.23333333333301</v>
+      </c>
+      <c r="K24">
+        <v>6.4686117407916299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -3477,8 +4005,14 @@
       <c r="I25">
         <v>8.9225692310120702E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>102.116666666667</v>
+      </c>
+      <c r="K25">
+        <v>11.8236930573372</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -3506,8 +4040,14 @@
       <c r="I26">
         <v>7.9047056064279697E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>113.166666666667</v>
+      </c>
+      <c r="K26">
+        <v>12.802497990714899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -3535,8 +4075,14 @@
       <c r="I27">
         <v>7.8332541053375698E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>110.583333333333</v>
+      </c>
+      <c r="K27">
+        <v>12.110076581188901</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -3564,8 +4110,14 @@
       <c r="I28">
         <v>8.1523065387358401E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>162.333333333333</v>
+      </c>
+      <c r="K28">
+        <v>3.7356127020727201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -3593,8 +4145,14 @@
       <c r="I29">
         <v>8.7461043472569805E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>100.883333333333</v>
+      </c>
+      <c r="K29">
+        <v>6.1205174996299796</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -3622,8 +4180,14 @@
       <c r="I30">
         <v>6.5986908558453405E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>148.6</v>
+      </c>
+      <c r="K30">
+        <v>32.150177267086498</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -3651,8 +4215,14 @@
       <c r="I31">
         <v>0.102569910409336</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>147.36666666666699</v>
+      </c>
+      <c r="K31">
+        <v>31.586827691552401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -3680,8 +4250,14 @@
       <c r="I32">
         <v>6.5644739016969697E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>162.38333333333301</v>
+      </c>
+      <c r="K32">
+        <v>4.7159723790779404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -3709,8 +4285,14 @@
       <c r="I33">
         <v>0.116066779376732</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>120.883333333333</v>
+      </c>
+      <c r="K33">
+        <v>20.082956486606701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -3738,8 +4320,14 @@
       <c r="I34">
         <v>7.0311709728691399E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>102.716666666667</v>
+      </c>
+      <c r="K34">
+        <v>33.973614720473002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -3775,15 +4363,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I35"/>
+      <selection activeCell="J1" sqref="J1:K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3811,8 +4399,14 @@
       <c r="I1">
         <v>0.104510772116784</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1">
+        <v>158.19999999999999</v>
+      </c>
+      <c r="K1">
+        <v>23.895819079737102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3840,8 +4434,14 @@
       <c r="I2">
         <v>0.110879840635229</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>135.816666666667</v>
+      </c>
+      <c r="K2">
+        <v>23.965718218269899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3869,8 +4469,14 @@
       <c r="I3">
         <v>7.9146834111229705E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>118.2</v>
+      </c>
+      <c r="K3">
+        <v>8.9457877598380193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3898,8 +4504,14 @@
       <c r="I4">
         <v>5.8303015849740902E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>141.53333333333299</v>
+      </c>
+      <c r="K4">
+        <v>6.2394770170526099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -3927,8 +4539,14 @@
       <c r="I5">
         <v>0.100587659437858</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>127.166666666667</v>
+      </c>
+      <c r="K5">
+        <v>16.583805319348599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -3956,8 +4574,14 @@
       <c r="I6">
         <v>6.7730090678823004E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>121.933333333333</v>
+      </c>
+      <c r="K6">
+        <v>6.2649594982030301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3985,8 +4609,14 @@
       <c r="I7">
         <v>7.7633086163984497E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>165.98333333333301</v>
+      </c>
+      <c r="K7">
+        <v>2.92558362519731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4014,8 +4644,14 @@
       <c r="I8">
         <v>6.8352326283467393E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>119.51666666666701</v>
+      </c>
+      <c r="K8">
+        <v>5.6583271968547999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4043,8 +4679,14 @@
       <c r="I9">
         <v>0.169569918977161</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>164.75</v>
+      </c>
+      <c r="K9">
+        <v>20.380802698717901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -4072,8 +4714,14 @@
       <c r="I10">
         <v>9.4952748013625105E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>104.2</v>
+      </c>
+      <c r="K10">
+        <v>30.643272826046601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -4101,8 +4749,14 @@
       <c r="I11">
         <v>9.9678512394699895E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>146.51666666666699</v>
+      </c>
+      <c r="K11">
+        <v>8.9546724223776302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -4130,8 +4784,14 @@
       <c r="I12">
         <v>8.5802046992524306E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>127.116666666667</v>
+      </c>
+      <c r="K12">
+        <v>28.627408738365499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -4159,8 +4819,14 @@
       <c r="I13">
         <v>6.1742801336157102E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>118.083333333333</v>
+      </c>
+      <c r="K13">
+        <v>7.8832404648081598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4188,8 +4854,14 @@
       <c r="I14">
         <v>0.11793470697769699</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>169.833333333333</v>
+      </c>
+      <c r="K14">
+        <v>3.87589974974283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4217,8 +4889,14 @@
       <c r="I15">
         <v>6.1991931383125698E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>108</v>
+      </c>
+      <c r="K15">
+        <v>11.6123838046767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -4246,8 +4924,14 @@
       <c r="I16">
         <v>9.5061011301673895E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>119.25</v>
+      </c>
+      <c r="K16">
+        <v>24.9695577365584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -4275,8 +4959,14 @@
       <c r="I17">
         <v>9.8263635390131707E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>150.71666666666701</v>
+      </c>
+      <c r="K17">
+        <v>15.7792952374968</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -4304,8 +4994,14 @@
       <c r="I18">
         <v>0.108977346463657</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>145.183333333333</v>
+      </c>
+      <c r="K18">
+        <v>8.8958029842428097</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -4333,8 +5029,14 @@
       <c r="I19">
         <v>9.5817354218213205E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>138.85</v>
+      </c>
+      <c r="K19">
+        <v>6.5037798657682799</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -4362,8 +5064,14 @@
       <c r="I20">
         <v>6.9034641353101903E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>166.25</v>
+      </c>
+      <c r="K20">
+        <v>2.6013360322231298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -4391,8 +5099,14 @@
       <c r="I21">
         <v>8.6492270654796699E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>139.36666666666699</v>
+      </c>
+      <c r="K21">
+        <v>6.9647214325318396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -4420,8 +5134,14 @@
       <c r="I22" s="1">
         <v>7.6365175857802503E-7</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>132.01666666666699</v>
+      </c>
+      <c r="K22">
+        <v>33.8393471040648</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -4449,8 +5169,14 @@
       <c r="I23">
         <v>8.5712010756245793E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>129.26666666666699</v>
+      </c>
+      <c r="K23">
+        <v>32.558092366277798</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -4478,8 +5204,14 @@
       <c r="I24">
         <v>8.6360844558475203E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>125.833333333333</v>
+      </c>
+      <c r="K24">
+        <v>16.802105060476102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -4507,8 +5239,14 @@
       <c r="I25">
         <v>9.1942881832324394E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>168.86666666666699</v>
+      </c>
+      <c r="K25">
+        <v>2.9998116701715101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -4536,8 +5274,14 @@
       <c r="I26">
         <v>6.5522079396538799E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>110.9</v>
+      </c>
+      <c r="K26">
+        <v>11.563677791593699</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -4565,8 +5309,14 @@
       <c r="I27">
         <v>7.8353000807920903E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>115.283333333333</v>
+      </c>
+      <c r="K27">
+        <v>16.0434702559361</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -4594,8 +5344,14 @@
       <c r="I28">
         <v>0.112062312897645</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>113.3</v>
+      </c>
+      <c r="K28">
+        <v>15.8042045467633</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -4623,8 +5379,14 @@
       <c r="I29">
         <v>8.7726190343449598E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>166.083333333333</v>
+      </c>
+      <c r="K29">
+        <v>3.0437023990175698</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -4652,8 +5414,14 @@
       <c r="I30">
         <v>5.9907114093025703E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>115.383333333333</v>
+      </c>
+      <c r="K30">
+        <v>5.5298624332865201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -4681,8 +5449,14 @@
       <c r="I31">
         <v>0.142475560272631</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>149.683333333333</v>
+      </c>
+      <c r="K31">
+        <v>32.886807239309199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -4710,8 +5484,14 @@
       <c r="I32">
         <v>0.118926000836655</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>148.94999999999999</v>
+      </c>
+      <c r="K32">
+        <v>32.366767325740803</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -4739,8 +5519,14 @@
       <c r="I33">
         <v>0.105527043597878</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <v>166.38333333333301</v>
+      </c>
+      <c r="K33">
+        <v>2.7927974352115701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -4768,8 +5554,14 @@
       <c r="I34">
         <v>6.6883332725703598E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>139.03333333333299</v>
+      </c>
+      <c r="K34">
+        <v>18.022553353466101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -4796,6 +5588,12 @@
       </c>
       <c r="I35">
         <v>0.112124339318828</v>
+      </c>
+      <c r="J35">
+        <v>119.116666666667</v>
+      </c>
+      <c r="K35">
+        <v>24.030412698563399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
print lines weggehaald bij de code
</commit_message>
<xml_diff>
--- a/results_others.xlsx
+++ b/results_others.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sander\git\AI-Negotiation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edward\Documents\GitHub\AI-Negotiation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="results_others" sheetId="1" r:id="rId1"/>
@@ -862,7 +862,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K28"/>
+      <selection activeCell="J1" sqref="J1:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1857,7 +1857,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K36"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3131,8 +3131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J1:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,10 +3166,10 @@
         <v>7.2866325140959504E-2</v>
       </c>
       <c r="J1">
-        <v>99.616666666666703</v>
+        <v>140.35</v>
       </c>
       <c r="K1">
-        <v>18.8185732871802</v>
+        <v>24.53</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3201,10 +3201,10 @@
         <v>8.9228562840130698E-2</v>
       </c>
       <c r="J2">
-        <v>119.916666666667</v>
+        <v>99.616666666666703</v>
       </c>
       <c r="K2">
-        <v>25.333231117843098</v>
+        <v>18.8185732871802</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3236,10 +3236,10 @@
         <v>9.6063945447810897E-2</v>
       </c>
       <c r="J3">
-        <v>102.783333333333</v>
+        <v>119.916666666667</v>
       </c>
       <c r="K3">
-        <v>8.5788302048482006</v>
+        <v>25.333231117843098</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -3271,10 +3271,10 @@
         <v>7.9684926114231405E-2</v>
       </c>
       <c r="J4">
-        <v>128.53333333333299</v>
+        <v>102.783333333333</v>
       </c>
       <c r="K4">
-        <v>7.8620881054927798</v>
+        <v>8.5788302048482006</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3306,10 +3306,10 @@
         <v>5.4595077057094203E-2</v>
       </c>
       <c r="J5">
-        <v>104.933333333333</v>
+        <v>128.53333333333299</v>
       </c>
       <c r="K5">
-        <v>10.881280250366</v>
+        <v>7.8620881054927798</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3341,10 +3341,10 @@
         <v>8.2950581080435598E-2</v>
       </c>
       <c r="J6">
-        <v>106.35</v>
+        <v>104.933333333333</v>
       </c>
       <c r="K6">
-        <v>8.35205242207069</v>
+        <v>10.881280250366</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3376,10 +3376,10 @@
         <v>7.36306490432556E-2</v>
       </c>
       <c r="J7">
-        <v>162.25</v>
+        <v>106.35</v>
       </c>
       <c r="K7">
-        <v>5.4169382808910704</v>
+        <v>8.35205242207069</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3411,10 +3411,10 @@
         <v>9.5662414263302104E-2</v>
       </c>
       <c r="J8">
-        <v>101.4</v>
+        <v>162.25</v>
       </c>
       <c r="K8">
-        <v>7.4017863166918101</v>
+        <v>5.4169382808910704</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3446,10 +3446,10 @@
         <v>6.8743524467712105E-2</v>
       </c>
       <c r="J9">
-        <v>143.80000000000001</v>
+        <v>101.4</v>
       </c>
       <c r="K9">
-        <v>24.130857943403999</v>
+        <v>7.4017863166918101</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3481,10 +3481,10 @@
         <v>9.69735037263878E-2</v>
       </c>
       <c r="J10">
-        <v>97.183333333333294</v>
+        <v>143.80000000000001</v>
       </c>
       <c r="K10">
-        <v>37.0054927973557</v>
+        <v>24.130857943403999</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3516,10 +3516,10 @@
         <v>8.86828121480156E-2</v>
       </c>
       <c r="J11">
-        <v>129.19999999999999</v>
+        <v>97.183333333333294</v>
       </c>
       <c r="K11">
-        <v>10.110910368239701</v>
+        <v>37.0054927973557</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3551,10 +3551,10 @@
         <v>7.4617564566123895E-2</v>
       </c>
       <c r="J12">
-        <v>104.51666666666701</v>
+        <v>129.19999999999999</v>
       </c>
       <c r="K12">
-        <v>13.011717882735001</v>
+        <v>10.110910368239701</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3586,10 +3586,10 @@
         <v>7.3877841283894893E-2</v>
       </c>
       <c r="J13">
-        <v>101.666666666667</v>
+        <v>104.51666666666701</v>
       </c>
       <c r="K13">
-        <v>7.4188643350986601</v>
+        <v>13.011717882735001</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3621,10 +3621,10 @@
         <v>5.1615923988169998E-2</v>
       </c>
       <c r="J14">
-        <v>165.1</v>
+        <v>101.666666666667</v>
       </c>
       <c r="K14">
-        <v>4.5349864051521998</v>
+        <v>7.4188643350986601</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3656,10 +3656,10 @@
         <v>0.106746411558655</v>
       </c>
       <c r="J15">
-        <v>79.75</v>
+        <v>165.1</v>
       </c>
       <c r="K15">
-        <v>14.240816249696801</v>
+        <v>4.5349864051521998</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3691,10 +3691,10 @@
         <v>5.6563249896642701E-2</v>
       </c>
       <c r="J16">
-        <v>115.683333333333</v>
+        <v>79.75</v>
       </c>
       <c r="K16">
-        <v>18.450567642424499</v>
+        <v>14.240816249696801</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3726,10 +3726,10 @@
         <v>0.12475332172355399</v>
       </c>
       <c r="J17">
-        <v>128.38333333333301</v>
+        <v>115.683333333333</v>
       </c>
       <c r="K17">
-        <v>7.0086911340441702</v>
+        <v>18.450567642424499</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3761,10 +3761,10 @@
         <v>7.8940631526247099E-2</v>
       </c>
       <c r="J18">
-        <v>127.216666666667</v>
+        <v>128.38333333333301</v>
       </c>
       <c r="K18">
-        <v>7.7088803440053599</v>
+        <v>7.0086911340441702</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3796,10 +3796,10 @@
         <v>7.5883391521368498E-2</v>
       </c>
       <c r="J19">
-        <v>129.01666666666699</v>
+        <v>127.216666666667</v>
       </c>
       <c r="K19">
-        <v>9.2415635676621992</v>
+        <v>7.7088803440053599</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3831,10 +3831,10 @@
         <v>0.10837382889507299</v>
       </c>
       <c r="J20">
-        <v>163.05000000000001</v>
+        <v>129.01666666666699</v>
       </c>
       <c r="K20">
-        <v>3.4268382423136101</v>
+        <v>9.2415635676621992</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3866,10 +3866,10 @@
         <v>9.2861550710241395E-2</v>
       </c>
       <c r="J21">
-        <v>125.166666666667</v>
+        <v>163.05000000000001</v>
       </c>
       <c r="K21">
-        <v>8.7936160716635303</v>
+        <v>3.4268382423136101</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3901,10 +3901,10 @@
         <v>8.5370411397977297E-2</v>
       </c>
       <c r="J22">
-        <v>126.916666666667</v>
+        <v>125.166666666667</v>
       </c>
       <c r="K22">
-        <v>31.6523979152498</v>
+        <v>8.7936160716635303</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3936,10 +3936,10 @@
         <v>9.1267267801604005E-2</v>
       </c>
       <c r="J23">
-        <v>104.133333333333</v>
+        <v>126.916666666667</v>
       </c>
       <c r="K23">
-        <v>9.05438683202539</v>
+        <v>31.6523979152498</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3971,10 +3971,10 @@
         <v>6.3118491336210794E-2</v>
       </c>
       <c r="J24">
-        <v>161.23333333333301</v>
+        <v>104.133333333333</v>
       </c>
       <c r="K24">
-        <v>6.4686117407916299</v>
+        <v>9.05438683202539</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -4006,10 +4006,10 @@
         <v>8.9225692310120702E-2</v>
       </c>
       <c r="J25">
-        <v>102.116666666667</v>
+        <v>161.23333333333301</v>
       </c>
       <c r="K25">
-        <v>11.8236930573372</v>
+        <v>6.4686117407916299</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -4041,10 +4041,10 @@
         <v>7.9047056064279697E-2</v>
       </c>
       <c r="J26">
-        <v>113.166666666667</v>
+        <v>102.116666666667</v>
       </c>
       <c r="K26">
-        <v>12.802497990714899</v>
+        <v>11.8236930573372</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -4076,10 +4076,10 @@
         <v>7.8332541053375698E-2</v>
       </c>
       <c r="J27">
-        <v>110.583333333333</v>
+        <v>113.166666666667</v>
       </c>
       <c r="K27">
-        <v>12.110076581188901</v>
+        <v>12.802497990714899</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -4111,10 +4111,10 @@
         <v>8.1523065387358401E-2</v>
       </c>
       <c r="J28">
-        <v>162.333333333333</v>
+        <v>110.583333333333</v>
       </c>
       <c r="K28">
-        <v>3.7356127020727201</v>
+        <v>12.110076581188901</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -4146,10 +4146,10 @@
         <v>8.7461043472569805E-2</v>
       </c>
       <c r="J29">
-        <v>100.883333333333</v>
+        <v>162.333333333333</v>
       </c>
       <c r="K29">
-        <v>6.1205174996299796</v>
+        <v>3.7356127020727201</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -4181,10 +4181,10 @@
         <v>6.5986908558453405E-2</v>
       </c>
       <c r="J30">
-        <v>148.6</v>
+        <v>100.883333333333</v>
       </c>
       <c r="K30">
-        <v>32.150177267086498</v>
+        <v>6.1205174996299796</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -4216,10 +4216,10 @@
         <v>0.102569910409336</v>
       </c>
       <c r="J31">
-        <v>147.36666666666699</v>
+        <v>148.6</v>
       </c>
       <c r="K31">
-        <v>31.586827691552401</v>
+        <v>32.150177267086498</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -4251,10 +4251,10 @@
         <v>6.5644739016969697E-2</v>
       </c>
       <c r="J32">
-        <v>162.38333333333301</v>
+        <v>147.36666666666699</v>
       </c>
       <c r="K32">
-        <v>4.7159723790779404</v>
+        <v>31.586827691552401</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -4286,10 +4286,10 @@
         <v>0.116066779376732</v>
       </c>
       <c r="J33">
-        <v>120.883333333333</v>
+        <v>162.38333333333301</v>
       </c>
       <c r="K33">
-        <v>20.082956486606701</v>
+        <v>4.7159723790779404</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -4321,10 +4321,10 @@
         <v>7.0311709728691399E-2</v>
       </c>
       <c r="J34">
-        <v>102.716666666667</v>
+        <v>120.883333333333</v>
       </c>
       <c r="K34">
-        <v>33.973614720473002</v>
+        <v>20.082956486606701</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -4354,6 +4354,12 @@
       </c>
       <c r="I35">
         <v>9.7225012872900099E-2</v>
+      </c>
+      <c r="J35">
+        <v>102.716666666667</v>
+      </c>
+      <c r="K35">
+        <v>33.973614720473002</v>
       </c>
     </row>
   </sheetData>
@@ -4365,8 +4371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K35"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>